<commit_message>
Clean-up/Updates done on dvplan which some of them related to functional coverage mapping
Signed-off-by: dd-baoshan <baoshan.mak@dolphin.fr>
</commit_message>
<xml_diff>
--- a/cv32e40p/docs/VerifPlans/Simulation/micro_architecture/CV32E40P_FPU_register_file.xlsx
+++ b/cv32e40p/docs/VerifPlans/Simulation/micro_architecture/CV32E40P_FPU_register_file.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t xml:space="preserve">Requirement Location</t>
   </si>
@@ -108,6 +108,36 @@
   </si>
   <si>
     <t xml:space="preserve">Functional Coverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corev_rand_fp* tests</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RISCV_coverage_pkg/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RISCV_coverage__1/&lt;f-instr&gt;_s_cg</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1) functional covergae for f-ext Is captured by using ISA cov model from Imperas ref model
+2) bit toggling is not captured due to large impact of sim performance when such cp is enabled</t>
   </si>
   <si>
     <t xml:space="preserve">Race between integer and floating point RF access</t>
@@ -125,16 +155,8 @@
 - fp load uses f_i as rD, the next integer instruction uses x_i as a source</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">corev_fp_instr_data_fwd_test
+    <t xml:space="preserve">corev_rand_fp_instr_data_fwd_test
 </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Zfinx</t>
@@ -149,7 +171,12 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">corev_fp_instr_data_fwd_test  </t>
+    <t xml:space="preserve">corev_rand_fp_instr_data_fwd_test
+corev_rand_fp_instr_mlt_cyc_test
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updates made on 2024_0311</t>
   </si>
 </sst>
 </file>
@@ -159,7 +186,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -191,26 +218,53 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -239,57 +293,61 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -301,6 +359,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB4C7DC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -309,33 +427,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="47.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="38.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="38.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="32.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="40.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="25.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="49.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="1" width="10.69"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -344,7 +463,7 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -353,107 +472,121 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+    <row r="2" customFormat="false" ht="46.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="I2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="11" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" s="11" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="8" t="s">
+    <row r="3" customFormat="false" ht="180.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
+      <c r="I3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
+      <c r="I4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Revert "Clean-up/Updates done on dvplan which some of them related to functional coverage mapping"
This reverts commit 594cb7db79ed63517f276b1c887b0a5e8d8addf3.
</commit_message>
<xml_diff>
--- a/cv32e40p/docs/VerifPlans/Simulation/micro_architecture/CV32E40P_FPU_register_file.xlsx
+++ b/cv32e40p/docs/VerifPlans/Simulation/micro_architecture/CV32E40P_FPU_register_file.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t xml:space="preserve">Requirement Location</t>
   </si>
@@ -108,36 +108,6 @@
   </si>
   <si>
     <t xml:space="preserve">Functional Coverage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">corev_rand_fp* tests</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">RISCV_coverage_pkg/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">RISCV_coverage__1/&lt;f-instr&gt;_s_cg</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">1) functional covergae for f-ext Is captured by using ISA cov model from Imperas ref model
-2) bit toggling is not captured due to large impact of sim performance when such cp is enabled</t>
   </si>
   <si>
     <t xml:space="preserve">Race between integer and floating point RF access</t>
@@ -155,8 +125,16 @@
 - fp load uses f_i as rD, the next integer instruction uses x_i as a source</t>
   </si>
   <si>
-    <t xml:space="preserve">corev_rand_fp_instr_data_fwd_test
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">corev_fp_instr_data_fwd_test
 </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Zfinx</t>
@@ -171,12 +149,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">corev_rand_fp_instr_data_fwd_test
-corev_rand_fp_instr_mlt_cyc_test
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Updates made on 2024_0311</t>
+    <t xml:space="preserve">corev_fp_instr_data_fwd_test  </t>
   </si>
 </sst>
 </file>
@@ -186,7 +159,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -218,41 +191,21 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB4C7DC"/>
-        <bgColor rgb="FFCCCCFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -260,13 +213,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -293,61 +239,57 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -359,66 +301,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB4C7DC"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -427,34 +309,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="17.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="47.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="38.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="32.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="40.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="25.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="49.49"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="1" width="10.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="38.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -463,7 +344,7 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -472,121 +353,107 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="46.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" s="11" customFormat="true" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="180.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+      <c r="F3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>